<commit_message>
dropping to 2 domains
</commit_message>
<xml_diff>
--- a/namelist_files_and_local_scripts/time_series_station_files_2_dom.xlsx
+++ b/namelist_files_and_local_scripts/time_series_station_files_2_dom.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/SD_Mines_WRF_REALTIME/namelist_files_and_local_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F55C4C-245B-E449-8E57-E4A4B41E1776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3DCE8C-6AA0-7C44-9FB9-88B227EBCD3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9920" yWindow="5840" windowWidth="33600" windowHeight="19860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Station ID</t>
   </si>
@@ -43,9 +54,6 @@
     <t>KBFF</t>
   </si>
   <si>
-    <t>KSIB</t>
-  </si>
-  <si>
     <t>KTOR</t>
   </si>
   <si>
@@ -58,12 +66,6 @@
     <t>K4DG</t>
   </si>
   <si>
-    <t>K4MC</t>
-  </si>
-  <si>
-    <t>KBPP</t>
-  </si>
-  <si>
     <t>KCDR</t>
   </si>
   <si>
@@ -85,30 +87,15 @@
     <t>KIEN</t>
   </si>
   <si>
-    <t>KLEM</t>
-  </si>
-  <si>
-    <t>KMIS</t>
-  </si>
-  <si>
     <t>KPHP</t>
   </si>
   <si>
     <t>KPIR</t>
   </si>
   <si>
-    <t>KVTN</t>
-  </si>
-  <si>
-    <t>KY22</t>
-  </si>
-  <si>
     <t>KCUT</t>
   </si>
   <si>
-    <t>KEFC</t>
-  </si>
-  <si>
     <t>KRAP</t>
   </si>
   <si>
@@ -124,101 +111,74 @@
     <t>KUNR</t>
   </si>
   <si>
-    <t>KW43</t>
+    <t>Buffalo, SD</t>
+  </si>
+  <si>
+    <t>Douglas, WY</t>
+  </si>
+  <si>
+    <t>Converse Co Arpt, WY</t>
+  </si>
+  <si>
+    <t>Gillette, WY</t>
+  </si>
+  <si>
+    <t>Faith, SD</t>
+  </si>
+  <si>
+    <t>Chadron, NE</t>
+  </si>
+  <si>
+    <t>Torrington, WY</t>
+  </si>
+  <si>
+    <t>Scottsbluff, NE</t>
   </si>
   <si>
     <t>Alliance, NE</t>
   </si>
   <si>
-    <t>Scottsbluff, NE</t>
-  </si>
-  <si>
-    <t>Sibley Peak, WY</t>
-  </si>
-  <si>
-    <t>Torrington, WY</t>
+    <t>Rapid City NWS, SD</t>
+  </si>
+  <si>
+    <t>Rapid City NEXRAD, SD</t>
+  </si>
+  <si>
+    <t>Gordon, NE</t>
+  </si>
+  <si>
+    <t>Hettinger, ND</t>
+  </si>
+  <si>
+    <t>Pine Ridge, SD</t>
+  </si>
+  <si>
+    <t>Pierre, SD</t>
+  </si>
+  <si>
+    <t>Philip, SD</t>
+  </si>
+  <si>
+    <t>Custer, SD</t>
+  </si>
+  <si>
+    <t>Rapid City Airport, SD</t>
+  </si>
+  <si>
+    <t>Ellsworth AFB, SD</t>
   </si>
   <si>
     <t>Munich, ND</t>
   </si>
   <si>
-    <t>Buffalo, SD</t>
-  </si>
-  <si>
-    <t>Douglas, WY</t>
-  </si>
-  <si>
-    <t>Moorcroft, WY</t>
-  </si>
-  <si>
-    <t>Bowman, ND</t>
-  </si>
-  <si>
-    <t>Chadron, NE</t>
-  </si>
-  <si>
-    <t>Custer, SD</t>
-  </si>
-  <si>
-    <t>Faith, SD</t>
-  </si>
-  <si>
-    <t>Converse Co Arpt, WY</t>
-  </si>
-  <si>
-    <t>Belle Fourche, SD</t>
-  </si>
-  <si>
-    <t>Gillette, WY</t>
-  </si>
-  <si>
-    <t>Gordon, NE</t>
-  </si>
-  <si>
-    <t>Hettinger, ND</t>
-  </si>
-  <si>
-    <t>Pine Ridge Arpt, SD</t>
-  </si>
-  <si>
-    <t>Lemmon, SD</t>
-  </si>
-  <si>
-    <t>Mission, SD</t>
-  </si>
-  <si>
-    <t>Philip Airport Sd</t>
-  </si>
-  <si>
-    <t>Pierre Arpt, SD</t>
-  </si>
-  <si>
-    <t>Rapid City Arpt, SD</t>
-  </si>
-  <si>
-    <t>Ellsworth AFB, SD</t>
-  </si>
-  <si>
     <t>Clyde Ice Field, SD</t>
-  </si>
-  <si>
-    <t>Rapid City NEXRAD, SD</t>
-  </si>
-  <si>
-    <t>Rapid City NWS, SD</t>
-  </si>
-  <si>
-    <t>Miller Field Arpt, NE</t>
-  </si>
-  <si>
-    <t>Hulett, WY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,11 +189,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -273,13 +228,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -583,18 +535,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="30.1640625" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
-    <col min="4" max="6" width="30.1640625" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -624,8 +573,8 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>35</v>
+      <c r="D2" t="s">
+        <v>34</v>
       </c>
       <c r="E2">
         <v>42.05</v>
@@ -644,8 +593,8 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>36</v>
+      <c r="D3" t="s">
+        <v>33</v>
       </c>
       <c r="E3">
         <v>41.871000000000002</v>
@@ -656,7 +605,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -664,19 +613,19 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>37</v>
+      <c r="D4" t="s">
+        <v>32</v>
       </c>
       <c r="E4">
-        <v>42.433</v>
+        <v>42.061</v>
       </c>
       <c r="F4">
-        <v>-105.033</v>
+        <v>-104.158</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -684,39 +633,39 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>38</v>
+      <c r="D5" t="s">
+        <v>45</v>
       </c>
       <c r="E5">
-        <v>42.061</v>
+        <v>48.666699999999999</v>
       </c>
       <c r="F5">
-        <v>-104.158</v>
+        <v>-98.834999999999994</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>39</v>
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
       </c>
       <c r="E6">
-        <v>48.666699999999999</v>
+        <v>45.603999999999999</v>
       </c>
       <c r="F6">
-        <v>-98.834999999999994</v>
+        <v>-103.54600000000001</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -724,19 +673,19 @@
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>40</v>
+      <c r="D7" t="s">
+        <v>27</v>
       </c>
       <c r="E7">
-        <v>45.603999999999999</v>
+        <v>42.75</v>
       </c>
       <c r="F7">
-        <v>-103.54600000000001</v>
+        <v>-105.383</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -744,19 +693,19 @@
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>41</v>
+      <c r="D8" t="s">
+        <v>31</v>
       </c>
       <c r="E8">
-        <v>42.75</v>
+        <v>42.837000000000003</v>
       </c>
       <c r="F8">
-        <v>-105.383</v>
+        <v>-103.098</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
@@ -764,19 +713,19 @@
       <c r="C9">
         <v>2</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>42</v>
+      <c r="D9" t="s">
+        <v>30</v>
       </c>
       <c r="E9">
-        <v>44.267000000000003</v>
+        <v>45.031999999999996</v>
       </c>
       <c r="F9">
-        <v>-104.95</v>
+        <v>-102.01900000000001</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -784,19 +733,19 @@
       <c r="C10">
         <v>2</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>43</v>
+      <c r="D10" t="s">
+        <v>28</v>
       </c>
       <c r="E10">
-        <v>46.186999999999998</v>
+        <v>42.795999999999999</v>
       </c>
       <c r="F10">
-        <v>-103.428</v>
+        <v>-105.38</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
@@ -804,421 +753,237 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>44</v>
+      <c r="D11" t="s">
+        <v>29</v>
       </c>
       <c r="E11">
-        <v>42.837000000000003</v>
+        <v>44.338999999999999</v>
       </c>
       <c r="F11">
-        <v>-103.098</v>
+        <v>-105.542</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>45</v>
+      <c r="D12" t="s">
+        <v>37</v>
       </c>
       <c r="E12">
-        <v>43.732999999999997</v>
+        <v>42.805999999999997</v>
       </c>
       <c r="F12">
-        <v>-103.611</v>
+        <v>-102.175</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>46</v>
+      <c r="D13" t="s">
+        <v>38</v>
       </c>
       <c r="E13">
-        <v>45.031999999999996</v>
+        <v>46.017000000000003</v>
       </c>
       <c r="F13">
-        <v>-102.01900000000001</v>
+        <v>-102.65</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>47</v>
+      <c r="D14" t="s">
+        <v>39</v>
       </c>
       <c r="E14">
-        <v>42.795999999999999</v>
+        <v>43.021000000000001</v>
       </c>
       <c r="F14">
-        <v>-105.38</v>
+        <v>-102.518</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>48</v>
+      <c r="D15" t="s">
+        <v>41</v>
       </c>
       <c r="E15">
-        <v>44.734000000000002</v>
+        <v>44.051000000000002</v>
       </c>
       <c r="F15">
-        <v>-103.86199999999999</v>
+        <v>-101.601</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>49</v>
+      <c r="D16" t="s">
+        <v>40</v>
       </c>
       <c r="E16">
-        <v>44.338999999999999</v>
+        <v>44.381</v>
       </c>
       <c r="F16">
-        <v>-105.542</v>
+        <v>-100.286</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>50</v>
+      <c r="D17" t="s">
+        <v>42</v>
       </c>
       <c r="E17">
-        <v>42.805999999999997</v>
+        <v>43.732999999999997</v>
       </c>
       <c r="F17">
-        <v>-102.175</v>
+        <v>-103.611</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>51</v>
+      <c r="D18" t="s">
+        <v>43</v>
       </c>
       <c r="E18">
-        <v>46.014000000000003</v>
+        <v>44.042999999999999</v>
       </c>
       <c r="F18">
-        <v>-102.655</v>
+        <v>-103.054</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>52</v>
+      <c r="D19" t="s">
+        <v>44</v>
       </c>
       <c r="E19">
-        <v>43.021000000000001</v>
+        <v>44.133000000000003</v>
       </c>
       <c r="F19">
-        <v>-102.518</v>
+        <v>-103.1</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>53</v>
+      <c r="D20" t="s">
+        <v>46</v>
       </c>
       <c r="E20">
-        <v>45.918999999999997</v>
+        <v>44.482999999999997</v>
       </c>
       <c r="F20">
-        <v>-102.10599999999999</v>
+        <v>-103.783</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>54</v>
+      <c r="D21" t="s">
+        <v>36</v>
       </c>
       <c r="E21">
-        <v>43.033000000000001</v>
+        <v>44.133000000000003</v>
       </c>
       <c r="F21">
-        <v>-100.617</v>
+        <v>-102.833</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>55</v>
+      <c r="D22" t="s">
+        <v>35</v>
       </c>
       <c r="E22">
-        <v>44.051000000000002</v>
+        <v>44.072699999999998</v>
       </c>
       <c r="F22">
-        <v>-101.601</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>19</v>
-      </c>
-      <c r="B23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23">
-        <v>44.381</v>
-      </c>
-      <c r="F23">
-        <v>-100.286</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>20</v>
-      </c>
-      <c r="B24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24">
-        <v>44.042999999999999</v>
-      </c>
-      <c r="F24">
-        <v>-103.054</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>21</v>
-      </c>
-      <c r="B25" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25">
-        <v>44.133000000000003</v>
-      </c>
-      <c r="F25">
-        <v>-103.1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>23</v>
-      </c>
-      <c r="B26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26">
-        <v>44.482999999999997</v>
-      </c>
-      <c r="F26">
-        <v>-103.783</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27">
-        <v>44.133000000000003</v>
-      </c>
-      <c r="F27">
-        <v>-102.833</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E28">
-        <v>44.072699999999998</v>
-      </c>
-      <c r="F28">
         <v>-103.211</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E29">
-        <v>42.878</v>
-      </c>
-      <c r="F29">
-        <v>-100.55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30">
-        <v>2</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30">
-        <v>44.6629</v>
-      </c>
-      <c r="F30">
-        <v>-104.568</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E31">
-        <v>45.933</v>
-      </c>
-      <c r="F31">
-        <v>-102.167</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F31">
-    <sortCondition ref="C2:C31"/>
-    <sortCondition ref="B2:B31"/>
-  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixing 2-domain station list
</commit_message>
<xml_diff>
--- a/namelist_files_and_local_scripts/time_series_station_files_2_dom.xlsx
+++ b/namelist_files_and_local_scripts/time_series_station_files_2_dom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/SD_Mines_WRF_REALTIME/namelist_files_and_local_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3DCE8C-6AA0-7C44-9FB9-88B227EBCD3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A82B0C-26A0-6740-B40C-C7BEB051F452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3580" yWindow="980" windowWidth="33600" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Station ID</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>Clyde Ice Field, SD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -535,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:C22"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -983,6 +986,11 @@
         <v>-103.211</v>
       </c>
     </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
patch to UPP script
</commit_message>
<xml_diff>
--- a/namelist_files_and_local_scripts/time_series_station_files_2_dom.xlsx
+++ b/namelist_files_and_local_scripts/time_series_station_files_2_dom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/SD_Mines_WRF_REALTIME/namelist_files_and_local_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A82B0C-26A0-6740-B40C-C7BEB051F452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A89CAB-2C84-394C-8B75-57EBE1FAFCCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="980" windowWidth="33600" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Station ID</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t>Clyde Ice Field, SD</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -538,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -986,11 +983,6 @@
         <v>-103.211</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C23" t="s">
-        <v>47</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
adding meteogram upgrade script.
</commit_message>
<xml_diff>
--- a/namelist_files_and_local_scripts/time_series_station_files_2_dom.xlsx
+++ b/namelist_files_and_local_scripts/time_series_station_files_2_dom.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/SD_Mines_WRF_REALTIME/namelist_files_and_local_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A89CAB-2C84-394C-8B75-57EBE1FAFCCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4CE354-856F-2F42-8156-66A45C624DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="980" windowWidth="33600" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -538,7 +541,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -565,425 +568,430 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="E2">
-        <v>42.05</v>
+        <v>43.732999999999997</v>
       </c>
       <c r="F2">
-        <v>-102.8</v>
+        <v>-103.611</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="E3">
-        <v>41.871000000000002</v>
+        <v>44.042999999999999</v>
       </c>
       <c r="F3">
-        <v>-103.593</v>
+        <v>-103.054</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="E4">
-        <v>42.061</v>
+        <v>44.133000000000003</v>
       </c>
       <c r="F4">
-        <v>-104.158</v>
+        <v>-103.1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E5">
-        <v>48.666699999999999</v>
+        <v>44.482999999999997</v>
       </c>
       <c r="F5">
-        <v>-98.834999999999994</v>
+        <v>-103.783</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E6">
-        <v>45.603999999999999</v>
+        <v>44.133000000000003</v>
       </c>
       <c r="F6">
-        <v>-103.54600000000001</v>
+        <v>-102.833</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E7">
-        <v>42.75</v>
+        <v>44.072699999999998</v>
       </c>
       <c r="F7">
-        <v>-105.383</v>
+        <v>-103.211</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E8">
-        <v>42.837000000000003</v>
+        <v>45.603999999999999</v>
       </c>
       <c r="F8">
-        <v>-103.098</v>
+        <v>-103.54600000000001</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E9">
-        <v>45.031999999999996</v>
+        <v>42.75</v>
       </c>
       <c r="F9">
-        <v>-102.01900000000001</v>
+        <v>-105.383</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E10">
-        <v>42.795999999999999</v>
+        <v>42.837000000000003</v>
       </c>
       <c r="F10">
-        <v>-105.38</v>
+        <v>-103.098</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E11">
-        <v>44.338999999999999</v>
+        <v>45.031999999999996</v>
       </c>
       <c r="F11">
-        <v>-105.542</v>
+        <v>-102.01900000000001</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E12">
-        <v>42.805999999999997</v>
+        <v>42.795999999999999</v>
       </c>
       <c r="F12">
-        <v>-102.175</v>
+        <v>-105.38</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E13">
-        <v>46.017000000000003</v>
+        <v>44.338999999999999</v>
       </c>
       <c r="F13">
-        <v>-102.65</v>
+        <v>-105.542</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E14">
-        <v>43.021000000000001</v>
+        <v>42.805999999999997</v>
       </c>
       <c r="F14">
-        <v>-102.518</v>
+        <v>-102.175</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E15">
-        <v>44.051000000000002</v>
+        <v>46.017000000000003</v>
       </c>
       <c r="F15">
-        <v>-101.601</v>
+        <v>-102.65</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E16">
-        <v>44.381</v>
+        <v>43.021000000000001</v>
       </c>
       <c r="F16">
-        <v>-100.286</v>
+        <v>-102.518</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E17">
-        <v>43.732999999999997</v>
+        <v>44.051000000000002</v>
       </c>
       <c r="F17">
-        <v>-103.611</v>
+        <v>-101.601</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E18">
-        <v>44.042999999999999</v>
+        <v>44.381</v>
       </c>
       <c r="F18">
-        <v>-103.054</v>
+        <v>-100.286</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E19">
-        <v>44.133000000000003</v>
+        <v>42.05</v>
       </c>
       <c r="F19">
-        <v>-103.1</v>
+        <v>-102.8</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E20">
-        <v>44.482999999999997</v>
+        <v>41.871000000000002</v>
       </c>
       <c r="F20">
-        <v>-103.783</v>
+        <v>-103.593</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E21">
-        <v>44.133000000000003</v>
+        <v>42.061</v>
       </c>
       <c r="F21">
-        <v>-102.833</v>
+        <v>-104.158</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E22">
-        <v>44.072699999999998</v>
+        <v>48.666699999999999</v>
       </c>
       <c r="F22">
-        <v>-103.211</v>
+        <v>-98.834999999999994</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F22">
+      <sortCondition descending="1" ref="C1:C22"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changing the number of time series files
</commit_message>
<xml_diff>
--- a/namelist_files_and_local_scripts/time_series_station_files_2_dom.xlsx
+++ b/namelist_files_and_local_scripts/time_series_station_files_2_dom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/SD_Mines_WRF_REALTIME/namelist_files_and_local_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4CE354-856F-2F42-8156-66A45C624DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7D81FA-B225-E948-B4AA-57D3A98ADA04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="980" windowWidth="33600" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13100" yWindow="9220" windowWidth="33600" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -541,7 +541,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -568,402 +568,402 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="E2">
-        <v>43.732999999999997</v>
+        <v>45.603999999999999</v>
       </c>
       <c r="F2">
-        <v>-103.611</v>
+        <v>-103.54600000000001</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="E3">
-        <v>44.042999999999999</v>
+        <v>42.75</v>
       </c>
       <c r="F3">
-        <v>-103.054</v>
+        <v>-105.383</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E4">
-        <v>44.133000000000003</v>
+        <v>42.05</v>
       </c>
       <c r="F4">
-        <v>-103.1</v>
+        <v>-102.8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E5">
-        <v>44.482999999999997</v>
+        <v>41.871000000000002</v>
       </c>
       <c r="F5">
-        <v>-103.783</v>
+        <v>-103.593</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E6">
-        <v>44.133000000000003</v>
+        <v>42.837000000000003</v>
       </c>
       <c r="F6">
-        <v>-102.833</v>
+        <v>-103.098</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E7">
-        <v>44.072699999999998</v>
+        <v>43.732999999999997</v>
       </c>
       <c r="F7">
-        <v>-103.211</v>
+        <v>-103.611</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E8">
-        <v>45.603999999999999</v>
+        <v>45.031999999999996</v>
       </c>
       <c r="F8">
-        <v>-103.54600000000001</v>
+        <v>-102.01900000000001</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E9">
-        <v>42.75</v>
+        <v>42.795999999999999</v>
       </c>
       <c r="F9">
-        <v>-105.383</v>
+        <v>-105.38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E10">
-        <v>42.837000000000003</v>
+        <v>44.338999999999999</v>
       </c>
       <c r="F10">
-        <v>-103.098</v>
+        <v>-105.542</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E11">
-        <v>45.031999999999996</v>
+        <v>42.805999999999997</v>
       </c>
       <c r="F11">
-        <v>-102.01900000000001</v>
+        <v>-102.175</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E12">
-        <v>42.795999999999999</v>
+        <v>46.017000000000003</v>
       </c>
       <c r="F12">
-        <v>-105.38</v>
+        <v>-102.65</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E13">
-        <v>44.338999999999999</v>
+        <v>43.021000000000001</v>
       </c>
       <c r="F13">
-        <v>-105.542</v>
+        <v>-102.518</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E14">
-        <v>42.805999999999997</v>
+        <v>44.051000000000002</v>
       </c>
       <c r="F14">
-        <v>-102.175</v>
+        <v>-101.601</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E15">
-        <v>46.017000000000003</v>
+        <v>44.381</v>
       </c>
       <c r="F15">
-        <v>-102.65</v>
+        <v>-100.286</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E16">
-        <v>43.021000000000001</v>
+        <v>44.042999999999999</v>
       </c>
       <c r="F16">
-        <v>-102.518</v>
+        <v>-103.054</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E17">
-        <v>44.051000000000002</v>
+        <v>44.133000000000003</v>
       </c>
       <c r="F17">
-        <v>-101.601</v>
+        <v>-103.1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E18">
-        <v>44.381</v>
+        <v>44.482999999999997</v>
       </c>
       <c r="F18">
-        <v>-100.286</v>
+        <v>-103.783</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E19">
-        <v>42.05</v>
+        <v>42.061</v>
       </c>
       <c r="F19">
-        <v>-102.8</v>
+        <v>-104.158</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E20">
-        <v>41.871000000000002</v>
+        <v>44.133000000000003</v>
       </c>
       <c r="F20">
-        <v>-103.593</v>
+        <v>-102.833</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E21">
-        <v>42.061</v>
+        <v>44.072699999999998</v>
       </c>
       <c r="F21">
-        <v>-104.158</v>
+        <v>-103.211</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -989,7 +989,7 @@
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F22">
-      <sortCondition descending="1" ref="C1:C22"/>
+      <sortCondition ref="A1:A22"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
changing metar station order
</commit_message>
<xml_diff>
--- a/namelist_files_and_local_scripts/time_series_station_files_2_dom.xlsx
+++ b/namelist_files_and_local_scripts/time_series_station_files_2_dom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/SD_Mines_WRF_REALTIME/namelist_files_and_local_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7D81FA-B225-E948-B4AA-57D3A98ADA04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C548A4A-73AF-4D4D-ACC6-4F2F72084ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13100" yWindow="9220" windowWidth="33600" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="980" windowWidth="33600" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -541,7 +541,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -568,102 +568,102 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E2">
-        <v>45.603999999999999</v>
+        <v>44.072699999999998</v>
       </c>
       <c r="F2">
-        <v>-103.54600000000001</v>
+        <v>-103.211</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="E3">
-        <v>42.75</v>
+        <v>44.042999999999999</v>
       </c>
       <c r="F3">
-        <v>-105.383</v>
+        <v>-103.054</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E4">
-        <v>42.05</v>
+        <v>44.133000000000003</v>
       </c>
       <c r="F4">
-        <v>-102.8</v>
+        <v>-103.1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E5">
-        <v>41.871000000000002</v>
+        <v>44.133000000000003</v>
       </c>
       <c r="F5">
-        <v>-103.593</v>
+        <v>-102.833</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E6">
-        <v>42.837000000000003</v>
+        <v>44.482999999999997</v>
       </c>
       <c r="F6">
-        <v>-103.098</v>
+        <v>-103.783</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -688,308 +688,308 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E8">
-        <v>45.031999999999996</v>
+        <v>43.021000000000001</v>
       </c>
       <c r="F8">
-        <v>-102.01900000000001</v>
+        <v>-102.518</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="E9">
-        <v>42.795999999999999</v>
+        <v>44.051000000000002</v>
       </c>
       <c r="F9">
-        <v>-105.38</v>
+        <v>-101.601</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="E10">
-        <v>44.338999999999999</v>
+        <v>48.666699999999999</v>
       </c>
       <c r="F10">
-        <v>-105.542</v>
+        <v>-98.834999999999994</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="E11">
-        <v>42.805999999999997</v>
+        <v>45.603999999999999</v>
       </c>
       <c r="F11">
-        <v>-102.175</v>
+        <v>-103.54600000000001</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E12">
-        <v>46.017000000000003</v>
+        <v>42.837000000000003</v>
       </c>
       <c r="F12">
-        <v>-102.65</v>
+        <v>-103.098</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E13">
-        <v>43.021000000000001</v>
+        <v>44.381</v>
       </c>
       <c r="F13">
-        <v>-102.518</v>
+        <v>-100.286</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="E14">
-        <v>44.051000000000002</v>
+        <v>44.338999999999999</v>
       </c>
       <c r="F14">
-        <v>-101.601</v>
+        <v>-105.542</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E15">
-        <v>44.381</v>
+        <v>45.031999999999996</v>
       </c>
       <c r="F15">
-        <v>-100.286</v>
+        <v>-102.01900000000001</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="E16">
-        <v>44.042999999999999</v>
+        <v>42.795999999999999</v>
       </c>
       <c r="F16">
-        <v>-103.054</v>
+        <v>-105.38</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E17">
-        <v>44.133000000000003</v>
+        <v>42.805999999999997</v>
       </c>
       <c r="F17">
-        <v>-103.1</v>
+        <v>-102.175</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E18">
-        <v>44.482999999999997</v>
+        <v>46.017000000000003</v>
       </c>
       <c r="F18">
-        <v>-103.783</v>
+        <v>-102.65</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E19">
-        <v>42.061</v>
+        <v>42.05</v>
       </c>
       <c r="F19">
-        <v>-104.158</v>
+        <v>-102.8</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E20">
-        <v>44.133000000000003</v>
+        <v>41.871000000000002</v>
       </c>
       <c r="F20">
-        <v>-102.833</v>
+        <v>-103.593</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E21">
-        <v>44.072699999999998</v>
+        <v>42.061</v>
       </c>
       <c r="F21">
-        <v>-103.211</v>
+        <v>-104.158</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="E22">
-        <v>48.666699999999999</v>
+        <v>42.75</v>
       </c>
       <c r="F22">
-        <v>-98.834999999999994</v>
+        <v>-105.383</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F22">
-      <sortCondition ref="A1:A22"/>
+      <sortCondition descending="1" ref="C1:C22"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>